<commit_message>
Get daily reddit data: Tue Apr  1 08:12:15 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C509"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3542 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1joq2yu</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Pink/Chrome with almond shape 💞</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dvh6cybh6se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1jopzh2</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>chrome frenchies… yay or nay ?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ih0eyzzf6se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1jopdgc</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>April Fool's Day Clown Nail Art 🎭🎨💅</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jopdgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1joo92h</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Any nail design ideas if one hand is has long nails and the other is short?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joo92h</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1joo37w</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I finally had time to do my own nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmd9civzr5se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1jontb1</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Has anyone used proxy services from Korea for nail polishes?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jontb1/has_anyone_used_proxy_services_from_korea_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1jonn4y</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Hibiscus Colour Pop!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jonn4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1jonfnf</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Kaleidoscope dimension continued. . .</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jonfnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1jon1ul</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First time getting hard gel. What do you think?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qb5e7ml9g5se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1jomj56</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>is it reasonable to go back to get these redone?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jomj56</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1jom51j</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Now if only I could find a foundation that suited my skin tone this well! 😩</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jom51j</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1jommxd</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Serving romantic vibes with a touch of sparkle! 💖✨</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aznrcoyb5se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1jom3gs</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>🤍💅</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktji6e8h65se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1jokn88</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>So what should I do</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x18lijss4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1jom1jo</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Love me a tigers eye</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o5ijy6ix55se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1johr95</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Any ideas for a better base color and good green for a french tip? (inspo in desc)</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1johr95</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1joj1nt</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Aries nails inspo help</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i58ty3fhe4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1jojfur</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Acrylic causing dent in nail bed. What's happening?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clolf381i4se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1jojgiv</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Toothless the Dragon Nails</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h9owk77i4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1joky03</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Custom mixes</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1joky03/custom_mixes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1jolixh</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Why do my nails break so easily?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ivocmvx05se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1jolnoh</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Welp.</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k9100h725se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1jolm9f</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>milky white nails 🥛✨</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jolm9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1jolipy</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Anyone else use glitter to cover up mistakes and chips? 😬</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exu8jdqv05se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1jolhq5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Just want to share my graduation set!</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jolhq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1jolcig</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Lavender French tips. Does your technician clean your cuticles before going on tips?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ublkbjw9z4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1jokvlr</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>I quit doing nails，ep2</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jokvlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1jokvky</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Eid Mubarak! ✨ (Done at the beginning of Ramadan)</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mcumj0uu4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1jokqmu</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Fresh set for spring😌</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eicbo92mt4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1jojy4y</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>How to protect natural nails while having gel on your nails?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jojy4y/how_to_protect_natural_nails_while_having_gel_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1jojtjl</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>New spring/ Easter themed nails!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk6s0yqfl4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1jojpal</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>bulky gel polish</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jojpal</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1jojoy5</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>I think my nail tech scammed me</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jojoy5/i_think_my_nail_tech_scammed_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1jojgor</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Opi not drying</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jojgor/opi_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1jojc0x</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Obsessed with my new set 😍</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prk10sa4h4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1joixv4</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>help w fixing my natural nails!!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joixv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1joiqp8</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Nails came off please tell me where I went wrong</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joiqp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1joikz6</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Oldie but a Goodie</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joikz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1joh7u1</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Disco nails!! 🪩🪩🪩🪩</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joh7u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1jogonw</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Whenever I need a hit of dopamine I just look at my nails😍</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8a6wb1kfu3se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1jogoas</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Burning and bruising after gel mani</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n81rf8f9u3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1jogif1</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>April birthstone nails-Diamond</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jogif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1jog7uq</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I like the length</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3knk2xwqq3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1jog6yb</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Painting my own reusable press ons</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jog6yb/painting_my_own_reusable_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1jofxy3</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>This is a bad day</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy3byyalo3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1jofo2f</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Tipping?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jofo2f/tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1jofm7p</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Tortoise Print Nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jofm7p/tortoise_print_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1jofgmq</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Is it okay to buff out nail ridges?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jofgmq/is_it_okay_to_buff_out_nail_ridges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1jofeac</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>first time doing acrylic</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jofeac</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1jof9ys</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Red is such a power move</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qknd7mzmj3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1jof5km</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>My attempt at yellow long nails 🫣🥴</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wl57ppoi3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1jof2rq</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>My first portrait!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jof2rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1joe7lf</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Spring nails 🌹🌺🌼🦋🍓</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/btwcqlglb3se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1jodyws</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>✨ spring cinnaroll ✨</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fss8wjn93se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1jodxi8</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New blue chrome set 🥰</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zvjfeel93se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1jodntn</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Thoughts on this negative salon experience?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jodntn/thoughts_on_this_negative_salon_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1jodke4</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Nails damaged.</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jodke4</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1jnsxrf</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Finger nail is crooked</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t50tvmzeqxre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1jnza5t</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Loving these</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jnza5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1joa87h</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Evil Queen but make it Nail Art</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joa87h</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1joax4p</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Need help deciding what to do next!</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg99bfdon2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1jobqv6</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Nails split horizontally after press ons</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f49biofqt2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1jocxsd</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>orange creamsicle 🧡🕉️</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jocxsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1jocpsn</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3szhj4p03se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1jockdl</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Bunny Nails 🐰</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18k5tw7mz2se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1joc9ma</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>My nails are yellow!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1joc9ma/my_nails_are_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1joc768</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Tried builder gel on myself for the first time and love it</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joc768</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1jobu2w</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Mermaid Nails!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2u9nh27eu2se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1job15c</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Eyeshadow tips and tricks!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1job15c</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1joags7</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Frenchie 💅🏻</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joags7</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1joaacg</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>🥦 Painted Polish Broccoli Biology 💜</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joaacg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1joa3mz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Soap Nails 🫧</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dysir9uph2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1jo9t0w</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>This months nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo9t0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1jo96i1</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Press ons + builder gel</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo96i1/press_ons_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1jo8y0q</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo8y0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1jo8upx</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake Nails 🍓🍰</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo8upx</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1jnhnlt</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Should I cut my nails super short to eliminate damage?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5v5awly3vre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1jo7g2b</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Nail shapes for feminine hands</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo7g2b/nail_shapes_for_feminine_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1jo7phi</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Help! Getting nails to stay on</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo7phi/help_getting_nails_to_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1jo7zh0</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agbhr3om22se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1jo7xyp</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Alice in wonderland!! My fav is the bread and butterfly</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqic1zrb22se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1jo7xpm</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Proud of these!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvh71jg922se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1jo7nnj</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Airbrush &amp; Chrome</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc3nnam602se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1jo7h1v</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>April showers or sumn idk</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tizvedrqy1se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1jo45ez</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkmvrfqj91se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1jo4j3z</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Nails lifting with skin build up underneath</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbrlj0zkc1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1jo4kqy</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Where to find this nail filer?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo4kqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1jo5y2k</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Press-on glue allergy</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo5y2k/presson_glue_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1jo6wgz</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Easiest baby boomers</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6l331dku1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1jo2qg0</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Gel top coat help!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzed1zoox0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1jo24ec</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>ripping off fake nails?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo24ec/ripping_off_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1jo0q0x</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Did builder gel ruin my nail beds</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jo0q0x/did_builder_gel_ruin_my_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1jo73hf</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>got new manicure today.</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo73hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1jo6zsi</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Did some fun gyaru nails 🐆</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo6zsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1jo6v5v</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>favorite set</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo6v5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1jo6kqw</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>how much would you pay for this?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rubaw257s1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1jo6j5p</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Wizard of Oz nails!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo6j5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1jo60jv</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Bunnies!!!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72l058wyn1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1jo5qkn</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Coquette nails</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo5qkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1jo5oz0</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Blue Iridescent 😍✨️</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orzyrmcjl1se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1joqdzh</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>I started taking care of my nails. They’ve never been worse. What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joqdzh/i_started_taking_care_of_my_nails_theyve_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1joq8do</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Funny Feeling</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joq8do</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1joq1s7</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>First spring mani! I call it April Showers</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lwfpgdqg6se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1jopqw1</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Which European indie/boutique nail polishes you love?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jopqw1/which_european_indieboutique_nail_polishes_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1jopbeo</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>PSA maybe: don't store horseshoe magnet too close to nail polish while traveling?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jopbeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1jopagb</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Love my new mani! 🐸</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jopagb</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1jonyhq</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Is it normal for a broken nail to never heal properly?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jonyhq/is_it_normal_for_a_broken_nail_to_never_heal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1jonzhd</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Do you know a dupe for julep’s tali? I miss it so much🥺</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22k1fk3tq5se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1jomnsg</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>what nail shape do you think would look most flattering on my hands? (these are my natural length)</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jomnsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1jomtfk</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Riding Sleeping Bags Down the Stairs dupe?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jomtfk/riding_sleeping_bags_down_the_stairs_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1jolxw5</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>First attempt at a bow</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/daoivkux45se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1jolwj5</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Arcana Emissary of Inari</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jolwj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1jolo3u</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Favorite Orly Shade?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jolo3u/favorite_orly_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1joll71</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>March manis🥰</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joll71</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1jol19f</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>First nail polish mani in a very, very long time!</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qcu67baw4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1jokxcd</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Wrinkling tips</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jokxcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1jokfmi</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Emily de Molly - The God Project</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qrv52dyzq4se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1joka6p</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>🎊 Happy 14th Anniversary &amp; Indie Nail Polish Award Results 🥁</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joka6p/happy_14th_anniversary_indie_nail_polish_award/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1jok893</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Take Me to Your Leader 👽</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7odanw4p4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1jok4wb</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Kazuo Ishiguro ft. Flower Child</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqrjsr9ao4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1jok3ki</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Did the OPI Nail Envy original formula have different formulations for US and EU?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jok3ki/did_the_opi_nail_envy_original_formula_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1jojjza</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>ILNP Rewind swatches📼</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1fifwt1j4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1jojej7</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>ILNP Sirene (H) in two different lightings</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jojej7</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1joja49</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Having fun experimenting with a black/clear water marble!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joja49</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1joitbu</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Favorite and least favorite brands and why?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joitbu/favorite_and_least_favorite_brands_and_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1joioo2</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Delivered early instead of late for once</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygqbypt7b4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1joijw8</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>In 24 hours, I will buy the most upvoted polish commented. Any brand, any colour - no limitations! Go crazy</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joijw8/in_24_hours_i_will_buy_the_most_upvoted_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1joi2j4</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>I put off a big chop so life did it for me… made myself feel better with Hermès🧡</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joi2j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1joi1wx</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I tried the new magnet hack ❤️</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xouhhxdt54se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1joi218</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>DIY Kit for a Kid? Or custom colors I can order?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joi218/diy_kit_for_a_kid_or_custom_colors_i_can_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1johbct</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Cracked Polish Fairy Tale Fog 🧚 ✨</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1johbct</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1jogzzi</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>other glowy recs? 🌟🌟</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jogzzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1jogszj</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Customer Experience</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/zAduVVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1jogjp5</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Found my perfect elevated neutral 🎀✨</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jogjp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1jogapc</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Black Fire Opal 🖤🔥🌈</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x0dk4rqcr3se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1jog8qt</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Sat on this purchase for way too long!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jog8qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1jof9ah</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>That glow tho 🌟</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp2vlpehj3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1jof7yk</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Absolutely love this polish and formula 💙</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jof7yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1joew8l</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>What I wore in March!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joew8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1joew7g</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Does adding thinner to a quick dry formula change the quick drying property at all?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joew7g/does_adding_thinner_to_a_quick_dry_formula_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1joe04m</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Winter - Spring round up 🌸</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joe04m</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1jodz5g</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bye8a2x93se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1jodgk5</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Show Me Inside Your Helmer!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jodgk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1joci9j</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>TRANS VISIBILITY 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joci9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1jocgh4</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Can anyone identify this color?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jocgh4/can_anyone_identify_this_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1jobsxs</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Gimme!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jobsxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1jobn3z</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>The Juice is Loose (LynB)</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d45mwfys2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1jobcbj</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>“Soft” Nail Tips? Are they flimsy?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jobcbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1jo6gyn</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>CND Shellac Adhesion Issues</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo6gyn/cnd_shellac_adhesion_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1joarg4</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake 🍰🍓</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joarg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1joag2v</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Holy shit!!!!!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joag2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1joafe1</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Question about cuticle prep</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z62ol8kxj2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1joa99w</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>🥦 Painted Polish Broccoli Biology 💜</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joa99w</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1jo9ufs</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>March was all about magnetics 🧲 &amp; Victorian Varnish did not disappoint</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xm8zo33vf2se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1jo99ng</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>it's rewind time! ⏪️🩷 (gifted pr)</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xdlzk7gnb2se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1jo962n</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Gel Allergy</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo962n/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1jo922i</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>How many polishes do you have and how do you store them?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo922i/how_many_polishes_do_you_have_and_how_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1jo8zda</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Enchanted Aura🧚🏻💚💖</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo8zda</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1jo8y0j</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I 🩵 cvs glitters</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlw75zpg92se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1jo8ucw</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Clionadh Buttercup</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlb6b4fq82se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1jo8fps</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>KBShimmer: Amanita moment</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo8fps</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1jo7zcv</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>sally beauty polish thinners?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo7zcv/sally_beauty_polish_thinners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1jo7ip7</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>I love a subtle thermal</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo8ciqi5z1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1jo6zcn</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Need guidance with this chrome/gem look!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo6zcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1jo63pi</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Greek God/Goddess Collections?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo63pi/greek_godgoddess_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1jo5xi1</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Accidental Latte Vibes</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo5xi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1jo5poz</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>ILNP Sandbar Velvet</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo5poz</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1jo5h4i</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I was excited for the butterfly decal, and then it got squished…</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo5h4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1jo551u</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Current 2 Faves by OPI</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo551u</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1jo3tlm</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>I’m in love with this polish combo!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo3tlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1jo3sed</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>OMG it finally happened to me, I met another Laquerista in the wild!!!!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo3sed</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1jo3eiv</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Anybody here old enough to remember these?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8vxqvxi31se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1jo3b5k</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Stabbed Digits</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo3b5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1jo31o3</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>I have a new method of keeping my nails protected from acetone while still changing my polish every 2-3 days and I need someone to tell me if there’s anything wrong with it! (details in caption)</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpr5ld4g01se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1jo1wjg</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>My dog passed away last week. I wanted to use my first polish since his passing to honor him. This is Emily de Molly's When the Sun Leaves.</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qd0nq54q0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1jo1jo6</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>🖼💛Klimt: The Kiss💛🖼</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo1jo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1jnyzhp</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>First time using/buying indie polishes and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jnyzhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1jo0z8z</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Is there a way to make a sparse topper less sparse?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jo0z8z/is_there_a_way_to_make_a_sparse_topper_less_sparse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1jo0fjp</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Worth it for magnetics?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy3xe3qea0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1jnzycp</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>March Mani review!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jnzycp</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1jnzo21</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jnzo21/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1jnz6yk</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>I don't know you, but I kinda like the peeling effect of the water-based polish on oil-based ones</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0656rztbtzre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1jnz36k</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Funky Glitter Placement with Snoopy Accent 🐶</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jnz36k</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1jonmpx</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Hibiscus Colour Pop!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jonmpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1jomsz3</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>my bday nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv8phhknd5se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1jomec0</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>New set🐍</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jomec0</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1jom8mt</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Nails 🩵☁️</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jom8mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1jol9d5</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Black Fire Opal 🖤🔥🌈</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kf7thelcy4se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1jol1gs</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Today's work in Gel ♥️ love the color and just a detail 🫶🏻😻</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8yoh3kcw4se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1jojzox</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Floral Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jojzox</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1jojer4</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>This weeks design</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnsvrzsqh4se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1joi3cs</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I tried the new magnet hack ❤️</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qlefpxx564se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1johjqx</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>testing a new technique</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q92kat0k14se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1jogtwd</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37264ielv3se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1jogjdm</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>April Birthstone nails -Diamond</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jogjdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1jof8fn</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Simple animal print</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jof8fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1jocij6</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>First try at sculpting.</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sl4v6ss9z2se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1joahbh</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake 🍰🍓</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joahbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1jo871c</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I guess I went overboard with gold flakes and mylars</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dow3re342se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1jo5mtw</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Ready for April showers</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmymo9b2l1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1jo5h7n</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Transparent jelly nails without tips?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoy8at4vj1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1jo514x</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>first set :)</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5866e7hg1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1jo4vnj</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Daisies for Spring</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h306tggbf1se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1jo3j2r</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>maximalist custom set</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jo3j2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1jo2r96</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Cat Memorial Nails</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6426jxvx0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1jo2ojt</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Nailen Art</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzk7qqu7x0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1jo0mjc</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Fabulous</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1krsmalc0se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1jnyfe0</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Are acrylic paints safe for nail art?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jnyfe0/are_acrylic_paints_safe_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr  2 08:11:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C509"/>
+  <dimension ref="A1:C727"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9086,6 +9086,3712 @@
         </is>
       </c>
     </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1jpgrlj</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>tangled inspired nails i designed</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2exyslycscse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1jphnik</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Lotus nails 🪷</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jphnik</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1jphhhl</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Simplicity and brilliance never fail</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzlr3d1u0dse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1jpgzcv</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>So I finally nailed the (almost) perfect French tip with high arches and deep smile lines</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpgzcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1jpgyzj</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I need suggestions for hard Gel</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpgyzj/i_need_suggestions_for_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1jpgvqn</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Blooming Gel 😍</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpgvqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1jpfxzt</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/da6stsnajcse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1jpdqc8</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>second ever acrylic nail - please give me feedback!!</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpdqc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1jpf7q4</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Nail artist</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf02kknzbcse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1jpeoyy</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>New set 🤎</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpeoyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1jpeork</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Oh my goodness! I am so obsessed with these new nails ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flq2evxb7cse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1jpem8a</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Dollar store nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc0wefkk6cse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1jpegyi</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>MMA</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpegyi/mma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1jpecmh</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Bright Pink on natural nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpecmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1jpe6jw</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Beach and pearls</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpe6jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1jpdxfc</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Bridal cat eye- please help!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpdxfc/bridal_cat_eye_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1jpdoit</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Natural white</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdm0qushzbse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1jpdghv</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>products to improve nail health?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpdghv/products_to_improve_nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1jpda6u</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>How'd I do?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/530km54ewbse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1jpd7x3</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Black French Chrome 🖤</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpd7x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1jpcxxo</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Fresh fills</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpcxxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1jpcjwb</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Happy April! Another cat set :) April fools editions</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpcjwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1jpax1x</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Do I have an allergy already to gel?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpax1x/do_i_have_an_allergy_already_to_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1jpbpxv</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>How did you start to like the feeling of false nails?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpbpxv/how_did_you_start_to_like_the_feeling_of_false/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1jpbl7l</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Bikini Bottom Vibes</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ppgiwcfhbse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1jpb8u4</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>sparkles make everything better ✨</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpb8u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1jpb7jb</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Going to Salon</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpb7jb/going_to_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1jpartj</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>my sun and moon frenchie set has been super popular with customers! what do you think?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fm54tahabse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1jpa90t</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>My first soap nails</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ray6fe56bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1jpa8d0</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Spring has sprung!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpa8d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1jpa7xd</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>How nice they turned out 💕🌷</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5mgvjww5bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1jp9gsu</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Team cat eye for life!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9gsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1jpa2vu</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>First Spring Set 😊</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpa2vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1jpa294</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>The Gel Bottle vs Luminary? Or other options? Need help &amp; advice in choosing.</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpa294/the_gel_bottle_vs_luminary_or_other_options_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1jp9rl5</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Some press ons I made myself! What’re your thoughts</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9rl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1jp9qvi</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Vacation Nails - which is your favourite?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9qvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1jp9ppd</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>How can I fix the peeled skin &amp; white skin around nails/cuticle?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9ppd</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1jp9oe1</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Spring Nails - Hand painted</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1jp9lyd</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>DnD Barbie #640 - I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9fca7221bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1jp9hv8</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I did these myself!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16mb9lr70bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1jp918d</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I made this set of colorful nails, do you think it looked good? I'm still not convinced 🤨 (but it's okay progress)</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onqe0rzjwase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1jp8vas</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Unexpected fave</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp8vas</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1jp80wt</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Nail Glue Allergy</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp80wt/nail_glue_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1jp87x4</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>How do you remove fake gel nails? When I got them removed it left my names extremely damaged.</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp87x4/how_do_you_remove_fake_gel_nails_when_i_got_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1jp7wub</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>It’s giving spring vibes 🌷 My fave set yet!</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp7wub</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1jp7v4z</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Roses nails!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/now9ks3nnase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1jp7o7c</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Advice? Total newbie</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qiutju4mase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1jp7mbl</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>How was my first manicure? Also, how frequently should I be getting them?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp7mbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1jp3qug</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>What happened</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp3qug/what_happened/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1jp460r</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First Russian manicure</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sv4vpoww9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1jp77nu</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Ex nail biter- thank God for BIAB!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frn5e7ipiase1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1jp74yn</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>First time Acrylics!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0g08g65iase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1jp6qor</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>A moment for something simple but cute</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp6qor</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1jp6n2a</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Milky white&amp;Gold ombre</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q3byh6iease1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1jp6ksf</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Clear part of dip peeling off</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7533g5g1ease1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1jp6i25</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Anti depression nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btg3j3fhdase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1jp6gf6</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>How to trim nails by filing?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp6gf6/how_to_trim_nails_by_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1jp5vix</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>In home mani?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp5vix/in_home_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1jp5tbp</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Sculpted tips? I was going for a flower hedge look. It looked cooler in my head but I also kinda like it 😁😅</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp5tbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1jp5lai</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>update! got them redone and love the result!!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp5lai</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1jp5cdk</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Is this fixable :(</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp5cdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1jp569q</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Always like a classic ombré</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vs6y5a24ase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1jp4q11</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>What’s trending 2025?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp4q11/whats_trending_2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1jp48u8</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Mint green this time 💚</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdwtiabhx9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1jp3x9a</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Spring Ombré on Natural Nails</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecbqzo66v9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1jp3u98</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Fresh Set, Floral Mood</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp1h773ku9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1jp3g80</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Y'all be real with me, is this cute? Was it worth the 40min it took to do one hand? Should I add glitter, leave it as is, or soak it off 😮‍💨 I've never done nail art with gel polish before and I'm having doubts!!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp3g80</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1jp3eph</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Blue set! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp3eph</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1jp2yn7</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>What gel polish is the most similar to the color of bad n boujee by v beauty pure acrylic powder?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp2yn7/what_gel_polish_is_the_most_similar_to_the_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1jp2xkg</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Feeling classy!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp2xkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1jp2uil</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>French manicure</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp2uil/french_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1jp2rxc</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Fruit nails, I hate them (did them myself)</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp2rxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1jp2hq3</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Is my nail tech right?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di8d9g72l9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1jp2dkd</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>A still photo literally doesn’t even do them justice</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k98benn8k9se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1jp27k1</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Porcelain nails</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et8kk3a4j9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1jordl2</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>First time doing my nails at home with polygel, why does my cuticle region look so uneven ? and yes I know the shape is very bad lol.. Kindly give me some tips, I'll practice more :)</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jordl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1jouyr1</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Serious question: How do you actually compare nail salons before booking?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jouyr1/serious_question_how_do_you_actually_compare_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1jp1fo4</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Magnetic tip nails with XXXL tips</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bt21fild9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1joyxe1</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Can I get some help finding a particular style?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1joyxe1/can_i_get_some_help_finding_a_particular_style/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1jopuww</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>What am I supposed to do with this nail?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jy0rj1xbe6se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1jov7vt</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>My Spring Set 🌸🪻</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jov7vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1joxccs</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Natural nails curling under gel?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1joxccs/natural_nails_curling_under_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1joyp16</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Pain</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyyd5mg1u8se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1joz5ay</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>How do I keep my nail polish from chipping so quickly?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/derzxzf9x8se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1jp0fna</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>nail split at the cuticle</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h19avflg69se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1jp14ta</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Magnetic tip press ons</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jp14ta/magnetic_tip_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1jp1vhy</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Can you identify this opi red?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp1vhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1jp1q8t</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>How do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2rmua7qf9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1jp18gy</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Beere set 😍</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp18gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1jp154n</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Can I get my nails done with blistering around the cuticle?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ijk71khb9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1jp0td0</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>These press ons 😍</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp0td0</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1jp0rbe</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Pink w Chrome 💛</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp0rbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1jp0nfn</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>First time gluing rhinestones on nails 💎✨ What do you think of the result? I’m not completely convinced…</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt28vu9189se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1jp0m52</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>i spent 6 hours on these and i hate them so much 😭😭 my thumb already popped off help  idk what im doing wrong</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8w2hhvr79se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1jp06ju</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Is this break worth trying to fix or should I just cut my nail down?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ask6e7wm49se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1jozpmf</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>What do you charge for portrait nails?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u432bmq819se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1jozlc9</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jozlc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1jozaeo</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Forgot to post my birthday nails. Loving the iridescent 💜</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t78kw9p5y8se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1joz0to</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>I loved them</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e01cm4edw8se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1joyq6d</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Matcha Spring Vibes</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7pk1yf9u8se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1jpj4ql</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Help why is this happening?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkp2rc61mdse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1jpidmd</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Proximal nail fold is slightly detached??</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpidmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1jpibha</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Anyone else super disappointed in Lights Lacquer's recent changes?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d6ohovdbdse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1jph780</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Am I crazy or is Holotaco Glossy Taco better than Mooncat Speed Demon?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jph780/am_i_crazy_or_is_holotaco_glossy_taco_better_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1jpfsjh</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>My new favorite base and top coat?🌼</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpfsjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1jpfo17</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Slow Burn</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j8zkipdigcse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1jpfb3s</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>march mani roundup!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpfb3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1jpekdk</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Newbie to gels - the always peel. Should I use a builder get?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqqfucg56cse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1jpdxm2</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>The many faces of Dreamscape</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpdxm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1jpdoon</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>I did it - I finally found my perfect true red!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5ul14wfzbse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1jpdmmz</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Really proud of these!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpdmmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1jpcwal</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Maximizing my swatch sticks</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4ogo6aysbse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1jpcevb</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Kitty hypnosis</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/up8b5ianobse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1jpc9fg</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>What are your holy grail blues?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpc9fg/what_are_your_holy_grail_blues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1jpbyn7</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>White/silver shimmer</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpbyn7/whitesilver_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1jpbkel</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>They remind me of Dinosaurs</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpbkel</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1jpbgxc</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Going to Salon</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpbgxc/going_to_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1jpan5k</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>How can I fix the peeled skin &amp; white skin around nails &amp; cuticles</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpan5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1jpalr4</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Another 🏆🥇 for Clionadh 👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼👏🏼</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpalr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1jpagba</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Wavelength- Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpagba</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1jpaf48</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Swamp Gloss Ducks! Applied?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpaf48/swamp_gloss_ducks_applied/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1jpa0ip</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>High-key obsessed with chrome 😍</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gtrjfua4bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1jp9sm7</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>March Manis🩷🌼</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w78mwm5j2bse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1jp9hyr</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Absolutely obsessed but I don’t think pictures do it justice</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9hyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1jp8ze8</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>KBShimmer No Illusions</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp8ze8</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1jp8wgz</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Happy Egg-pril! 🐣</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49817c2ivase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1jp8oer</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Quick comparison</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp8oer</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1jp7y9z</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>March Mani Log</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp7y9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1jp7j52</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Let's Talk alongside Indomitable</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cykkmouakase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1jp7bzd</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>The quest for glowy blues: House of Hades vs Midnight Kiss and Flower Child</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp7bzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1jp78rh</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Fuzzy lizard toes!</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bssplgxiase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1jp780s</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>The Greenest March</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp780s</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1jp7390</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Weather This Together by LynB</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5dt2unshase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1jp6y5q</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Redid my nails, much happier with this!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp6y5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1jp6rqh</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Anyone have experience with swap polish packages getting lost?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jp6rqh/anyone_have_experience_with_swap_polish_packages/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1jp6pwy</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Dupe for Risquè Enamel Triangulum from the Doritos collection?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp6pwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1jp6oy3</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>March Mani Roundup 🍀</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp6oy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1jp6d36</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>How cute is the design my niece just did for me?!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp6d36</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1jp6a50</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Chunky glitters</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2rtm90xbase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1jp69ud</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Painting underside of nail swatches?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jp69ud/painting_underside_of_nail_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1jp687g</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I subconsciously matched my nails to my hard hat.</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x3pwhkibase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1jp5po9</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Thanks to those who stopped by&lt;3 This is the end results!!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp5po9</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1jp4oyo</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>ILNP Pool Party 🎉</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp4oyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1jp4mlp</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>what’s the maximum amount that you would pay for a discontinued bottle of nail polish?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jp4mlp/whats_the_maximum_amount_that_you_would_pay_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1jp4bxu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Mooncat skittle for April Fools' Day</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcdcikr3y9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1jp42ps</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Empty Journal💙</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp42ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1jp3vmf</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Matching with my Gnomie</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxwvjh3uu9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1jp3te9</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Fresh Set, Floral Mood</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cil93k9eu9se1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1jp3gyc</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>You probably recognize the feeling</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp3gyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1jp3d0f</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Magnetic reds comparison</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fx68lu4yo9se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1jp34br</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>teal glitter bomb craving satisfied</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jq3aebqgp9se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1jp2rj7</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Thought these would be easier than regular polish. They were not.</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jp2rj7/thought_these_would_be_easier_than_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1jp2lxc</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Hey ya'll, I'm currently live trying out this nail design for spring&lt;3 Pop by if you can!!!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.twitch.tv/tinywhalee</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1jp2lb5</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>rainbows make dopamine go brrrrrrr</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp2lb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1jp2h0z</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Handmade checkerboard decals</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp2h0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1jp2g84</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>ISO - Emily de Molly Cobalt Dream (or other neon blue)</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jp2g84/iso_emily_de_molly_cobalt_dream_or_other_neon_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1jp2ckq</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>"Topper Topper Topper" Little Ms Vicky probably</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp2ckq</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1jp212p</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>March nails 🐟🌸</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvyy81wvh9se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1joyg0r</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>This supplement basically completely stopped my nails from breaking, ever. And they used to break a lot! Highly recommend.</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1joyg0r/this_supplement_basically_completely_stopped_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1jp0qrm</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - 10 Drops (of spring🌷)</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp0qrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1jp0plx</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Sunset Skittle 🌅</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp0plx</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1jp0f70</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>March Manis 💅🏻</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp0f70</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1jp01r8</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Don’t you think the gold gives it a luxurious touch? I look at them and they seem to scream glamour!🥰</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9jccodo39se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1jozpsz</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Probably my best work 💅🏻</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jozpsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1joz8y7</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>How do I achieve this look?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joz8y7</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1joz6jh</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Ummm ... I guess I really liked blues this month?? 😂 New goal is 0 blue nails for April!!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joz6jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1joxtns</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Norpsilocin</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/naqcx6onn8se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1joxscr</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Dollar Tree $1.29 Polish 👀</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joxscr</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1joxlat</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Purple is a funny word to say</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bykf751m8se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1joxj0l</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Glass Nails Tutorial</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lc8mkdzjl8se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1joxe2a</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I adore Essie gel effect top coat but after 2-3 uses the shrinkage is insane. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joxe2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1jox93q</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Manis of March 🫶</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jox93q</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1jox72l</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I didn’t dupe myself</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jox72l</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1jox2tn</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Sparkly Green Beauty</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jox2tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1jowx2x</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>My magnetic setup</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jowx2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1jowsof</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>"I've had Indomitable on for 13 hours-</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jowsof</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1jowg0i</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>My new favorite polish!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jowg0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1jovx5s</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>these shades look even prettier in person !</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/woplamla98se1</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1jovpz3</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>What opi red is this?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jovpz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1jovcpq</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Glowy polish recommendations that aren’t a pink base with blue shimmer?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jovcpq/glowy_polish_recommendations_that_arent_a_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1jov99j</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Different color this week (my wife picked it out for me), with matching vest and cap, of course 😉. I hope my students like it!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jov99j</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1jov3cb</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Ground zero nails to developing at home nail care routine &amp; at home manicure.</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jov3cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1jouv1q</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>🍇 This Week’s Polish! 🍇</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jouv1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1jouuwx</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>My First PPU Order Came!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jouuwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1jouluv</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Cracked went all in for April Fools</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d3q0j37y7se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1jouc1v</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Not today satan ft my new snake 😍</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jouc1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1jotps6</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Hate it when I dupe myself🥲</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jotps6</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1jot8gf</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Thank you for loving me - Bee’s knees</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jot8gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1jorxb0</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jorxb0/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1jornmf</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Absolutely in love with my new magnetic set</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jornmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1jorivp</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Oh look I match. (Satire)</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jorivp</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1joqyvc</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Happy April Jewels Day</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1joqyvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1jpgy89</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpgy89</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1jpgpgp</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Got my dream nails!!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h0yav8orcse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1jpefpr</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Duck Nailss</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51bu70j25cse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1jpedvb</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Art History Nails !</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dblhohso4cse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1jpdm5l</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Close enough lol</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpdm5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1jpb3w1</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Nails ☁️🩵</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpb3w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1jpaznf</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>💜🌷spring nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpaznf</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1jpauje</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>If Spring Were Summer</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpauje</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1jpakmg</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I’m doing my own nails</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i4o2ezps8bse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1jp9rqi</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Vacation Nails - which is your favourite?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9rqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1jp9n3n</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Spring Nails - Hand painted</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp9n3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1jp92dd</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Kiss Impress in Portal</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d6qa8hswase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1jp8ubw</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Thinking about a greek summer</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeiffrm1vase1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1jp8kj4</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Pink and Green set</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgft4j7zsase1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1jp61lj</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>monet inspired nails 🌷</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp61lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1jp3tzb</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Snow White nails!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp3tzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1jp3duh</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Spring is in the air 🐝🍯</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jp3duh</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1jp0l6q</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>my sun and moon frenchie set has been super popular with customers ! what do you thin?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzmfm5hk79se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1jozor5</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Recents 🫶</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jozor5</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1jowqs1</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>5 hours doing my nails? Worth it!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jowqs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1jow4ne</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>The lustre I'm getting here... ✨🤩</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jow4ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1jovaw7</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My Spring Set 🌸</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jovaw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1jov15q</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Perfect for Spring</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0czsheu18se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1jots4g</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Amo el azul con blanco 💙🤍</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l23a3tjjq7se1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1jotna3</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Nail art design for concert</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jotna3/nail_art_design_for_concert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1jorlkk</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First attempt at stamping my natural nails. Not perfect but I'm happy.</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb87779p17se1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr  3 08:11:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C727"/>
+  <dimension ref="A1:C903"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12792,6 +12792,2998 @@
         </is>
       </c>
     </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1jqbzjb</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Swimmer nails</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqbzjb/swimmer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1jqblkv</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqblkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1jqb5ah</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>My momma said she knew what she was doing 😭</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqb5ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1jqb4db</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>This color but gel</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/026pr1subkse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1jqa6bp</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Woher kriege ich solche Press-Ons?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqa6bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1jq9bfg</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Cute 💗</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb5pf8besjse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1jq94mn</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>glittery goth press ons ✨</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq94mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1jq7spu</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Wish I'd done them all in blue</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avvz6a80ejse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1jq7qyh</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Miffy Space Cyber Core 🌠🐇</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq7qyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1jq7k08</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Ways to stop biting nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq7k08/ways_to_stop_biting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1jq7h09</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>First time extensions</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq7h09</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1jq7aug</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Is this normal for gel removal at a salon?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq7aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1jq77z2</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>…. This is bad right?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq77z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1jq76m3</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Is structure gel builder gel?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq76m3/is_structure_gel_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1jq67rt</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Chrome nails chat accidentally denied!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq67rt/chrome_nails_chat_accidentally_denied/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1jq5rv7</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq5rv7/nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1jq4fwr</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>I'm getting my nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq4fwr/im_getting_my_nails_done_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1jq4mjk</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Weigh in: do I ask for a fix?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmjxj72jmise1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1jq4xg5</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>beachy blue</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq4xg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1jq54lk</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Is it normal for the extension tip to be separated from the nail?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq54lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1jq3rtf</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Wanted to share my serotonin boost 😌</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq3rtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1jq41ow</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Should I say something?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcmoztnkhise1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1jq3hxy</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Need nail growth help</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq3hxy/need_nail_growth_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1jq3dr0</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Natural nails (after biting them my whole life)!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pinmeui2cise1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1jq3a75</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>April Nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq3a75</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1jq2tfm</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>What are these lines?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq2tfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1jq2svk</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1johy2cf7ise1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1jq1fkl</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Help me pick which orange/blue color combination!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1fkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1jq1kuv</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Chrome powder help!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1kuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1jq0nru</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Am I wrong to be upset I paid for these builder gel extensions?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq0nru</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1jq0lll</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Would this be a tapered almond or just almond?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1v2eehnqhse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1jq01a2</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>“I believe that happy girls are the prettiest girls." Audrey Hepburn 🎀✨️</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq01a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1jpwzvy</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Inconsistent results with press on nails (adhesive tabs). Please advise. Thank you!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpwzvy/inconsistent_results_with_press_on_nails_adhesive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1jpzd7m</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Wrong Chrome</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpzd7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1jpzp7m</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Cadbury mini egg nails for Easter</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpzp7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1jpypof</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Decided to try glue on nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh21y3gtchse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1jpyxn2</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Salon perfect press ons</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuus3q8fehse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1jpyvqr</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>My sister gave me a manicure, what do you think of them?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpyvqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1jpyvpk</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Pokémon Nail Art!@Corinasclaws</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjtlw2k1ehse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1jpyp3o</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Press ons from @LeFrenchTips on Etsy</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lb5re0pchse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1jpymzq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Hybrid press on manicure!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzgix9x8chse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1jpy75n</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>First time going to an independent nail tech😇</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpy75n</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1jpxkrh</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0jc38fum4hse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1jpxgb9</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I love this colour</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw2gxgrq3hse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1jpwc1t</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>(33)Boy Here, White dip powder base with all free style hand paint. I personally choose the designs and placements. Inspiration from my home decor and obsession of the mountains and the desert.</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpwc1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1jpx122</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Are these well done?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpx122</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1jpwvyw</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>I Need Suggestions Please...</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpwvyw/i_need_suggestions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1jpwst1</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Easter nailssss</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtohf5k3zgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1jpv7pd</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Miami nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpv7pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1jpv47o</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Cellular by Rogue Lacquer in my office lighting 💡🧫</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyfz5s77ngse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1jput8j</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>When am I ready for new nails?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jput8j/when_am_i_ready_for_new_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1jpuxs6</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>New acrylics !</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpuxs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1jpuk97</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>What is the difference between self painted nails vs getting yours done?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpuk97/what_is_the_difference_between_self_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1jpu9wn</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Check out my new nails! Inspo credit: @nailsbypaular</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpu9wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1jpu7cg</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Are these okay?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpu7cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1jpjop7</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>monet inspired nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpjop7</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1jpruxc</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Do press-ons cause flat nail beds?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpruxc/do_pressons_cause_flat_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1jpsqzn</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Painting a snow white set (1937 version) 😊</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t340skul6gse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1jpsihh</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>New Spring Nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpsihh</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1jprfgc</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Beautiful,like new😍</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz2m74pzwfse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1jppol9</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Spring is in the air ☺️🍓</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2qpx9j7kfse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1jpoonm</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I have been doing my natural nails at home since I'm 12. I'm 27 now, and this is my week's choice. I wanted a shiny nude but not so glittery, something like Romantic Ethereal ^~^</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d96ox6kmbfse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1jpoen6</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Did these myself. I can't pose my hands tho</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpoen6</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1jpod51</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Do you have any favorite style that you always do on your nails?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpod51/do_you_have_any_favorite_style_that_you_always_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1jpnxq8</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>First freestyle</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpnxq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1jpnx3y</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Been doing my own nails, but am still kind of new to this. What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg2knyj16fse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1jpnsx4</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Haven’t taken the time to do my nails in months, feel like myself again🥰</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79pqcfhz4fse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1jpnr7g</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Base coat for press ons?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpnr7g/base_coat_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1jpnllq</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Baby pink French tips with a bubble bath base🎀</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjfxzk253fse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1jpn3nu</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Struggling to find a nail tech who will work with me</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpn3nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1jpmrfh</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time getting my nails done. I’m obsessed.</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpmrfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1jpmo97</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Today's nails 💖</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2y2cvzeuese1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1jpllcp</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>please someone tell me how you do this middle cloth looking nail</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhrep1nsiese1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1jpkxl3</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>How to place a fake nail on crooked fingers.</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jpkxl3/how_to_place_a_fake_nail_on_crooked_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1jpklcc</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Mermaid nails🧜🏼‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nok3hq56ese1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1jpkjpy</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Caught my nail :,(</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpkjpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1jpk2xn</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>First time trying cat eye</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2766pb8zdse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1jpjvp1</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My first attempt at doing my own nails 🤣</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi99whufwdse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1jpjpj1</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Shorties for the first time in years 🌟</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p64id2n1udse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1jqc78a</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>New nail shape and some ILNP</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sm4v0ijokse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1jqbjgv</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Polish to match my chicken?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hth2uhmpgkse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1jqb4ha</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqb4ha/sally_hansen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1jq9lnz</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>HT wild child + HT made me ink?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq9lnz/ht_wild_child_ht_made_me_ink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1jq824g</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Cirque starfruit jelly</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc4kqc4fgjse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1jq7voc</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>First BKL and I GET IT NOW</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq7voc</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1jq7hry</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Advice for a guitarist</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq7hry/advice_for_a_guitarist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1jq79cc</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>LOVE LINEAR HOLOS</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qggz4ko59jse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1jq6stg</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Polishes that look like this fabric?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76ji0up35jse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1jq6s70</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Help with rubber base and gel</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq6s70/help_with_rubber_base_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1jq6owe</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Can I show you my new set? 🥺💅</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq6owe</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1jq6boi</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Nail Art without Gel</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq6boi/nail_art_without_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1jq5tn7</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>What’s your most anticipated upcoming release?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq5tn7/whats_your_most_anticipated_upcoming_release/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1jq5cry</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Enemies to Lovers for the Win!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57t67b9psise1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1jq59xq</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Me taking 5 business days to pick a design because of decision paralysis</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b73gezf1sise1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1jq594v</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Science but Make it Sparkle</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cjym3a3urise1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1jq551c</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Loving my lil jelly nails</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq551c</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1jq51z4</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Daughters of the Evening</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/exwk9s95qise1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1jq3v6w</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Confused about nail oil vs painting to encourage healthy growth</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq3v6w/confused_about_nail_oil_vs_painting_to_encourage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1jq3h7g</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Favorite brand for magnetics?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq3h7g/favorite_brand_for_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1jq33zb</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Thoughts on Sassy Sauce caviar?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9b6bx5kt9ise1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1jq2y98</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>EU alternative to PPU?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq2y98/eu_alternative_to_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1jq1z8o</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>LA Colors ravishing gown</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1z8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1jq1vt4</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Does anyone have both Strawberry Boba (Lights Lacquer) and Rosewater Jelly (Cirque Colors)?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq1vt4/does_anyone_have_both_strawberry_boba_lights/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1jq1qxg</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>HoloTaco's new flaky formula compared alongside Mooncat and Alchemy Lacquer: first impressions</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1qxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1jq1nwb</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>First BKL purchase!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/40mbr3guxhse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1jq1fpo</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>ILNP Poison - Velvet</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1fpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1jq1dch</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Refusing to do more than 3 coats so you add a topper to cover the dark spots ✨</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq1dch</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1jq0zty</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>I want to like it but I can't 😭</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8109c5jthse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1jpzeob</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Cadbury mini egg nails for Easter</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpzeob</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1jpz80a</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Help identifying baby polishes</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpz80a</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1jpyzn3</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Sacrificed the shiftiness for glow, ended up with a lovely blue at least</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpyzn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1jpya5c</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Grape nails for my bday :)))</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpya5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1jpxa3c</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨ VERSACE</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpxa3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1jpx35p</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Hilt - Clionadh</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpx35p</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1jpwv0g</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>A Change in Direction is STUNNING</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq4dx2rjzgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1jpwotw</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>First matte and first GITD!!!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpwotw</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1jpvyvy</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>How often do you keep your nails bare between manicures?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpvyvy/how_often_do_you_keep_your_nails_bare_between/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1jpvqaz</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Recent manis</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpvqaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1jpvoqe</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Are Cuticula and/or BCB cruelty free?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpvoqe/are_cuticula_andor_bcb_cruelty_free/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1jpvkxq</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Culture Shock is so vibrant!</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f997ter8qgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1jpv2jo</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Cellular by Rogue Lacquer in my office lighting 💡🧫</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zejl11pvmgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1jpuib7</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Orange-Pink Indie Shimmers</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r1dd2431jgse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1jpudwn</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>What's your favorite chocolate holo?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpudwn/whats_your_favorite_chocolate_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1jpu87a</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Essie gel couture in dress call</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lg3toh04hgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1jptzlr</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>It's been gloomy outside but cherry blossoms are doing their thing.</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x0z35redgse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1jptyfr</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>so glowy✨</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jptyfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1jptqkb</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>best/favorite latex/peel off protector?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jptqkb/bestfavorite_latexpeel_off_protector/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1jptiur</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Favorite Lurid Lacquer Polishes?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jptiur/favorite_lurid_lacquer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1jptfdl</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Mermaid Bait v They Would Know My Name One Day</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jptfdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1jpt5te</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>My ✨MCAT✨ manicure</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpt5te</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1jpsyq8</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Painted Polish Broccoli Biology (PPU 3/25)</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpe2zkb58gse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1jpso0r</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Fell for the hype</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wol647u06gse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1jpsm01</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Which sheer "your nails but better" polish would you recommend me? See caption</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpsm01</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1jps5eb</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Magnetic over Thermal (+vent warning)</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jps5eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1jps199</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Love a linear holo on this gloomy day!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jps199</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1jpry3b</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>What's on your destash list and why?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpry3b/whats_on_your_destash_list_and_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1jprmwd</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>I still do - Kathleen and co</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jprmwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1jprjh7</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Mooncat Dragon Scales 🐉</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n3rsziorxfse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1jprdv8</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>This is getting expensive.</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jprdv8/this_is_getting_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1jpraid</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Can you re-use swatch sticks when playing with combinations?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpraid/can_you_reuse_swatch_sticks_when_playing_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1jpr24c</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers skittle</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpr24c</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1jppw82</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Orly Breathable - You Had Me At Hydrangea</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jppw82</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1jppot8</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Nails Inc - Glowing my way: How to add more pink?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jppot8</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1jppn4k</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>🪼🐙 under the sea 🐙🪼</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jppn4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1jppjpf</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Confusing take: my husband said it looked like concrete.</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jppjpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1jppgl3</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>March Manis 🍀</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jppgl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1jppf78</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Springtime Mani 🦋🌸💐</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3ujfilaifse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1jppbcd</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Temu Horshoe Comparison</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/znwh7fmghfse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1jpp4gd</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Swatching Jellies, Glitters, and other Semi-Transparent Polishes - Question</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpp4gd/swatching_jellies_glitters_and_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1jpp0i1</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque Night Fever?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpp0i1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1jpoc4h</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Nettle and Briar</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpoc4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1jpo9yy</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Really sheer shimmer toppers?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpo9yy/really_sheer_shimmer_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1jpnxm0</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Happy little accident🥰💖🩵</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpnxm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1jpnljr</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Went to see the cherry blossoms in DC this past weekend, and painted my nails to match! 🌸</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpnljr</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1jpnh5k</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Vanessa Molina - Mystery Machine</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpnh5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1jpn0u7</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Nails are saving my life--what nails do psychologically</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jpn0u7/nails_are_saving_my_lifewhat_nails_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1jpcbon</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Foxfire vs. Aurora Unicorn Skin</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpcbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1jpkm4c</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Spring bulb mani! 🌷💐</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpkm4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1jpk8tw</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>ILNP - 'Get Cozy'</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpk8tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1jqbyjt</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>how do i fix this please help</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p7b9f0olkse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1jqber8</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>glittery purple!!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w1s1l8j5fkse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1jqb3fu</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Throwback Kitty set</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24s60j1jbkse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1jq9dra</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I love them🥰</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2kinnn1tjse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1jq1v2p</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>New set I did :’)</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2631lsy10ise1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1jq0ut9</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>All my favorite designs done by @ly_nailz north Georgia</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jq0ut9</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1jq007n</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Punk Bunnies 🖤🐰✨</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qmbgt7h8mhse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1jpy842</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Christmas 2024 nails :) chose a cute candy swirl and snowflake</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdtadpmd9hse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1jpy01q</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>My work on my clients</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpy01q</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1jpwxp9</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>First time trying to do a pattern 🌸</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t15rei20hse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1jpsplr</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Painting a snow white set (1937 version)</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e1tzgl5c6gse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1jps88u</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>First time trying nail art!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jps88u</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1jpr1dm</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Making your inspo come to life ✨ one set at a time 😊</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jpr1dm</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1jpqhym</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Day 7 nail update, only a little chipping</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlygm2u8qfse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1jppfg2</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Pompompurin 3d nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb8qzghcifse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1jplj0r</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>My friends nail art is next level</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jplj0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1jplbl8</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Spirited away 🥹</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jplbl8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr  4 08:11:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C903"/>
+  <dimension ref="A1:C1074"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15784,6 +15784,2913 @@
         </is>
       </c>
     </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1jr6bp0</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Mood: pink 🌸</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfyid09uurse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1jr68ic</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>IBD Hard Gel Question</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flwugndmtrse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1jr4qf5</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>summer beach vibes</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6462q76brse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1jr4m9w</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Spring Nails 🌸</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giu0rdav9rse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1jr3zow</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>happy with my new nails🍓 :3</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr3zow</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1jr3fup</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Before and After</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nr3sb0wwqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1jr3s0n</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Letter A French Mani Steps</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr3s0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1jr3qeb</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>April nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytvqvi320rse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1jr3o71</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Mediterranean Gel Mani</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpvu9zlezqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1jr325r</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>first time trying marble!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr325r</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1jqzsct</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Was this 80$ worth?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqzsct</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1jqy3qc</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>How much to tip when going back to redo a few nails?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqy3qc/how_much_to_tip_when_going_back_to_redo_a_few/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1jqzkcl</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>🍶🍋Lemons &amp; Porcelain🍋🍶</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqzkcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1jr2o9a</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>This is my idea for my Easter nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe20r9r8pqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1jqukth</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Celestial spring design</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqukth</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1jr2lay</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>skittle nails for Easter 🐇🐣</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr2lay</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1jquzzz</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Are these bubbles? Gel nails</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zeglz8fvose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1jqzqf0</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>My buddy’s insane nails</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqzqf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1jr2atu</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Destroyed nail from biting</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr2atu</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1jr2cwi</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Nail artist says lifting is my fault</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr2cwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1jr2hho</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>I asked for a bit of rock ‘n’ roll.</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f69si0pdnqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1jr2dgg</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>My press on set that I made.</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr2dgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1jr11tc</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Le Mini Macaroon Gel Nails</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jr11tc/le_mini_macaroon_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1jr1sm9</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>First time at a new place. Not sure how I feel</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr1sm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1jr1r2i</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Pastel cotton candy vibes</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azhpjuyegqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1jr1kj6</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Thought you ladies might appreciate my the nails ive made 🤗</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr1kj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1jr1ipj</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Cat Eyes 🤩</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8pa0mg67eqse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1jr19iv</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qecp209tbqse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1jr0z7j</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>took your guys advice!! &lt;33 these ones look SO much better, lets see how long they hold :)</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i57b7yy49qse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1jr0wne</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>First ever manicure!!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr0wne</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1jr0tx4</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>I love the color, but I might have to return and ask for a redo.</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr0tx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1jr0b7e</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I did my nails myself I think they look cute 🥹</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr94zm343qse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1jr055p</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>First time trying a bright colour</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c75lt94l1qse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1jqzrh6</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>First attempt at gel extensions</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdw1jjf2ypse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1jqz0yp</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>First time ever getting nails done!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqz0yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1jqykxh</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Sleek and simple. @v.rnish</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rm26e4mnpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1jqyil3</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Littles bees 🐝</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q16ap61npse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1jqychm</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>First time getting nails…advice?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3dys11mlpse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1jqyak7</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Looooove this set 💐♥️</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqyak7</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1jqxwgq</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Am I being a Karen?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7wzmgbyhpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1jqxl9j</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Ombre 🎀</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g5hzavbfpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1jqww9r</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Peely Base &amp; Treatment?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqww9r/peely_base_treatment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1jqwuch</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Vintage Liquid Euphoria in Euphoric</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqwuch</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1jqw3pq</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>First time trying xcoat tips</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqw3pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1jqvxo3</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>What grit nail file do you use?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqvxo3/what_grit_nail_file_do_you_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1jqvc9i</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Simple set</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqvc9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1jqv9yu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>I’m loving this new magnetic shimmer thing 😍</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/amgqpthgxose1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1jqva1c</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Beginner to nail art - recommendations on easily removable methods?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqva1c/beginner_to_nail_art_recommendations_on_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1jqv9zc</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>went for a more vampiresque look this time ❤️🧛🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5agzfjmgxose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1jquuu3</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Removing nail glue</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jquuu3/removing_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1jqunfh</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>First full face portrait</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6kqv2zusose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1jqufee</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>This stuff is amazing!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5gnywo9rose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1jquev7</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My fully natural nails, but both hands!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv7uubv5rose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1jqt3ru</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqt3ru/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1jqt9eh</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Bio gel vs acrylic sets</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqt9eh/bio_gel_vs_acrylic_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1jqu5la</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Are unpolished natural nails accepted here?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st4zq2ldpose1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1jqu2b8</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Cherry blossom mani</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqu2b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1jqtuww</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Please help find dupe again</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqtuww</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1jqtros</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>New Set!!!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yggaffjnmose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1jqtqp7</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Matchy matchy</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9bkytcgmose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1jqtnzb</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Learning new techniques💖</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bepo3mdxlose1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1jqthfr</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Tried my hand at a design!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3exr2t8okose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1jqstcw</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>i love blue 💎</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt0sh0u2gose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1jqssxe</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing 🌸💐❤️</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqssxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1jqsr31</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Talk to me 🖤🤍 what do we think?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqsr31</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1jqslyj</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Long nails appreciation</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohfi5tfqeose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1jqsjmh</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>My beautiful wedding set 🥰</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqsjmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1jqf3e3</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Spring Floral Shorties</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7juo5wmmlse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1jqng3m</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Thinking of going as short as @polished_yogi on Instagram at my next appointment</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqng3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1jqpfb7</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Why does my top coat look like this? Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n0l0il3tnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1jqpk9p</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>💋 short n sweet</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqpk9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1jqs3av</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Purple chrome on red 💖</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vpss207bose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1jqrwt0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Sometimes the best lighting is bathroom lighting 😅</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/064pdzpw9ose1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1jqrscp</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Are these darker streaks on my nail anything?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqrscp/are_these_darker_streaks_on_my_nail_anything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1jqrn69</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy7sgi328ose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1jqr4f4</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Acrylics vs Gel x vs sculpted gel?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqr4f4/acrylics_vs_gel_x_vs_sculpted_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1jqqz8s</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>I got the blues today</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxy53kdm3ose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1jqqw79</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>What do my nails say about me? 🤓(a silly fun game)</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqw79</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1jqqp3m</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Take Me To Mulberry Street by Catrice (feat. my cat) 🫐</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqp3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1jqqldq</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Current spring/bday set! 🌸🌸</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqldq</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1jqqi7d</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Time for a nail break… :(</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqqi7d/time_for_a_nail_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1jqqcps</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Press oms that i never got to wear</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqcps</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1jqqa40</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Switched my usual white French for a pop of red today 💋🍒</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqa40</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1jqp5mb</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Pinkalicious 💖</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqp5mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1jqowrd</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Requesting advice: shape of nails</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqowrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1jqorou</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Lavender nails for the spring 🌿</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81iqv2pgonse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1jqokc8</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Nude base w/ pink chrome</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqokc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1jqojp4</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>My own "hand"y work on my natural nails</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aorcmao6nnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1jqo2n7</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My vibe for the next month 💖</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqo2n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1jqnwmg</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>What do u guys think</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69swirvtinse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1jqngya</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Day 8 – This set is holding on pretty well!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/31cfvw6sfnse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1jqn5d0</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My latest press-on set</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqn5d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1jqmz49</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I am in love</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jgu0asgcnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1jqmtru</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Soooooo in love with this shade of green…….</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tlvxdjgbnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1jqmlz0</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Slowly getting back into doing my own nails again!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqmlz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1jq8dmt</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Why don't press-ons work for me?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jq8dmt/why_dont_pressons_work_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1jq8odi</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>My first cat eye! I'm gagging.</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwyi9uf5mjse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1jqmk7z</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My LDR Cherry Cola Inspired</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iese9akk9nse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1jqdpyr</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>need help!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqdpyr/need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1jqmhee</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Is there a safe way to use press on nails?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jqmhee/is_there_a_safe_way_to_use_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1jr54hl</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>First magnetic mani!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr54hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1jr1nog</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Magnetics hit the spot for the shiny things polish obsessed little gremlin in me</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/icpeh8phfqse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1jr16u4</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Tried to do flowers, but they look more like eggs 🍳</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr16u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1jqzxja</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Unmixed glitter</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhtva99mzpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1jqzirv</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Any product that will make my nail polish not peel off in one big sheet?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqzirv/any_product_that_will_make_my_nail_polish_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1jqzidf</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Another neon comparison</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqzidf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1jqza0x</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>March 🌸🪲🍀🐸🌱🧌 (sorry about the multiple posts y’all I was having technical issues posting from my phone 🥴😭)</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqza0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1jqysai</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Might be searching for unicorns, but maybe you all can help.</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqysai/might_be_searching_for_unicorns_but_maybe_you_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1jqyqxh</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>I think I have a type</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syjbim31ppse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1jqy536</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Olive and June “Can’t Lose” with Essie “Cosmic Chrome”</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1hwtysyjpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1jqxts0</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>!!SHAPING DILEMMA!!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqxts0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1jqxkp5</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>ahhhhhhhhhhhh</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf2nutd2fpse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1jqxdvt</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>💙🤍 jazz cup 🩵💜</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqxdvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1jqwos2</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Recommendations for best blue polish for pre-wedding gift</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqwos2/recommendations_for_best_blue_polish_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1jqwls6</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Why are some of the polishes on BKL shown without color?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqwls6/why_are_some_of_the_polishes_on_bkl_shown_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1jqwk13</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>App similar to Lacquergram?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqwk13/app_similar_to_lacquergram/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1jqwhn3</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Horizontal magnetic line</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqwhn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1jqwhg6</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Gloooooow for days</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqwhg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1jqw6nm</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Trying to create a chrome with no powder and no gel.</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqw6nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1jqvy5u</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Linear holo plus shimmer - send help</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqvy5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1jqvqlr</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Do I need to push back my cuticles?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs7jad1e0pse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1jqv9wt</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>QDTC’s and shrinkage</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqv9wt/qdtcs_and_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1jqug3h</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>I think these color shifts are addictive for my ADHD brain!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqug3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1jqu49p</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Nail art I made for Stray Kids concert in Brazil 🇧🇷</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqu2gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1jqtuip</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Damn Essie is so good for the price</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqtuip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1jqtsva</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Honeydew</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1kwq98wmose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1jqtq9t</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I love this color under the sun!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meppbqxdmose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1jqtmgn</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Unintended Dino Egg Nails - my attempt at glass nails that quickly went awry in a cool way</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqtmgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1jqtadb</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>✨Shimmer✨</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4pzyubbjose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1jqsq3x</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Help me match my nails to my dog?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j9ha8qhfose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1jqska7</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I think this is my perfect red polish</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmnndtlfeose1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1jqsfi5</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Is this what your bottle of eternal glow by PFD looks like? Or is mine wrong pigment/faded?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqsfi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1jqro7w</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>LynB - Poiesis</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqro7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1jqqxpp</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Gel palette dupes?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqqxpp/gel_palette_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1jqqo6v</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>That bathroom lighting though…</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r76mlmvg1ose1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1jqq8kr</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Sour Apple Rings vs. Emily de Molly - Behind Again</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqq8kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1jqq4sz</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Wish me luck with my interview tomorrow! 🤞🙏</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqq4sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1jqpnl1</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Who does the best neons?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqpnl1/who_does_the_best_neons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1jqpcke</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Current Favourite Manicure</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqpcke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1jqp5an</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>OPI - help!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5m6byc8rnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1jqp112</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Sparkliest red?!</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqp112/sparkliest_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1jqose5</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Pinkalicious 💖</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqose5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1jqockw</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>I *FEEL* like we should all start showing off our mistakes.</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xi9wmuplnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1jqo1q9</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>✨️💜Mental Health Ombré💜✨️</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqo1q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1jqnil1</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Gumdrop Mountains</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqnil1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1jqn4k0</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>I want to see your polishes that are so old there is no evidence they ever existed outside your stash!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqn4k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1jqmtpq</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>First Ever French Tips</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqmtpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1jqmqea</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Dupe for my cat's eyes?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8cyl4otanse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1jqm6dv</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Help! I’m buying a Jeep and want to find the perfect matching nail polish</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqm6dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1jqlmg9</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>My Wife Picks My Mani: Part 10</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqlmg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1jql9tx</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Spring has sprung!🪻🌅</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jql9tx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1jql55s</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>💐✨flower child ✨💐</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jql440</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1jqkv76</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Why is it so pretty!?!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqkv76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1jqknnk</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Honda Boost Blue Pearl</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqknnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1jqilno</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Nail polish that matches this vibe?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26vcevmjhmse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1jqi9c6</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Glossy Burgundy</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/LyEe85y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1jqfso0</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I have a question!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqfso0/i_have_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1jq519r</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>PPU &amp; AI Images</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jq519r/ppu_ai_images/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1jq5ngx</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Forever seeking the perfect IKB Yves blue nail polish??</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgwicbf6rise1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1jr4vp3</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Have you guys ever tried matte chrome? HIGHLY RECOMMEND - it looks like velvet 😍💅</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuvqmduwcrse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1jr1y4c</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>My latest set "I dream of unicorns" swipe to see the glow in the dark pieces. I'm actually obsessed with this set!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr1y4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1jqw829</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Craftsman-style set</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqw829</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1jqu2gd</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Nail art I made for Stray Kids concert in Brazil 🇧🇷</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqu2gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1jqtz09</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Cherry blossom mani</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqtz09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1jqoy81</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Day #3 of doing my gf's nails</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2uk6d2wpnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1jqmi09</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Lace French tips w/ gold and pearl accents</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hroilk59nse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1jqmb7u</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>My nail artist executes everything flawlessly 🐞</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqmb7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1jql5ht</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Short nails for work 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jql5ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1jqkml7</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0e9asi9wmse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1jqji0w</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Koi Nail Art</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqvrpii7omse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1jqfasa</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>What do you think? (I’m not a professional nail artist)</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqfasa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr  5 08:09:59 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1074"/>
+  <dimension ref="A1:C1268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18691,6 +18691,3304 @@
         </is>
       </c>
     </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1jryiui</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First world problem nail advice</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b469a1e94zse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1jryh7x</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Some spring nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gutped6p3zse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1jryb26</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>When spring &amp; easter is around the corner 🩷💜💙🩵💚</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jryb26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1jrxz77</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Saw this on Twitter - how cool is this?!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm2bpk50xyse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1jrxrk3</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Why did two of my nails turn green?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrxrk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1jrvv6d</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Online nail tech courses</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrvv6d/online_nail_tech_courses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1jrwv41</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>In Honor Of Minecraft Movie</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz4mgfqfjyse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1jrw8us</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Silver cat eye with nail art this time ⛓️‍💥🪩</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndttqbcxbyse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1jrvhd5</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>BF’s Toes</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrvhd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1jrvdsx</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Decided to take a break from polish and extensions</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/706nucu52yse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1jrupno</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>How much would you charge for this or are willing to pay? And what state you live in?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3qbs3s4vxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1jrukyp</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Minecraft nails-- girlie version 🩷💚</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrukyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1jruc9d</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>How do I put on fake nails with super glue long lasting?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jruc9d/how_do_i_put_on_fake_nails_with_super_glue_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1jru8le</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Nail Biters—What Treatments Help with Growth and Repair?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jru8le/nail_biterswhat_treatments_help_with_growth_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1jru817</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>when the base is perfect</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruacr2x2qxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1jrtz1y</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time ever! I am loving this color!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/058tdp0jnxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1jrtn1m</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Do I look beautiful?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxku6ee4kxse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1jrtat2</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Would you go back in to have these fixed?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrtat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1jrt0d7</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Now I’m worried</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrt0d7/now_im_worried/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1jrtlqs</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Best 3 hours ever spent</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ekwq6urjxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1jrtibw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Another simple little spring set for my brother-in-law’s girlfriend.</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh4gp30sixse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1jrthhf</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>My nails keep getting shorter and shorter! LOL!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0f725gjixse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1jrtf57</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Spring is Upon Us💚🌸🎀🤍💐🩷</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrtf57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1jrtcct</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>In my Gel X and Almond era</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jemicyz3hxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1jrt38d</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>First gel set I did on myself 🥰</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pccp0ikexse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1jrsvok</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Practice Set!!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvngilcjcxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1jrs2hq</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Silver Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9tdwqur4xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1jrs0gf</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>🤩</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrs0gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1jrrx5m</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Weekend Ready 🎊</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrrx5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1jrrsna</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>my newest set!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrrsna</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1jrrrwn</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Do any press-on nail brands make extremely short nails?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrrrwn/do_any_presson_nail_brands_make_extremely_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1jrrpp9</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Starry night</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7iojjird1xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1jrrm4w</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Celestial nails for my birthday</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nylmhtwg0xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1jrpaq0</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Thoughts on these?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqqn08rsfwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1jrpbjb</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Can someone tell me what my nail tech did?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrpbjb/can_someone_tell_me_what_my_nail_tech_did/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1jrrkok</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>🎀🤍</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mi5q9a30xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1jrrbbq</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Cutesy</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx1xqlekxwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1jrrb3t</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>My first time doing my nails with more than just basic color - feedback?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrrb3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1jrratt</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>i paid $159 for this.. was it worth it?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrratt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1jrr73p</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>How do we feel about these for spring?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qt7fs0kwwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1jrqlik</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Pink nails feet 🦶</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s5sojt3rwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1jrq19c</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Anyone else keep a folder of their sets so they are ready to show off at any time? 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrq19c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1jrpydb</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61sz0knflwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1jrpumq</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Color help</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hzx17gikwse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1jrpltf</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Easter egg nails 🐣</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckxs9s9eiwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1jrpbkq</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Hmm</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1jkfrgzfwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1jrpahy</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>My friend does it every time!!😍</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrpahy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1jrp7k5</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Strawberry Glaze</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrp7k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1jrp72d</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>How long does it take to do press ons?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe2t64ozewse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1jrozdb</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Best tool for even thin lines?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrozdb/best_tool_for_even_thin_lines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1jroxbh</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Easter Nails - not done by me</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxjer7xocwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1jrovjy</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Valentines day nails</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8cxpp5acwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1jrouch</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>cotton candy nails 💅 🍭</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrouch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1jrosjd</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>I really liked this set</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1e5e2blbwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1jroqbt</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Acrylic and regular polish?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jroqbt/acrylic_and_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1jron4j</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me the most?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jron4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1jrolyg</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>“Cuticle” help.  Issues NO MaTTER what.</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrolyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1jrohvv</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>spooky for spring...brilliant</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22mwkx349wse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1jrognx</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Cat eye w polka dots!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrognx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1jroecz</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Blue and green</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jroecz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1jro9ln</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Icy blue cat eye nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jro9ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1jro8wk</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>First attempt at strawberry milk nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jro8wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1jrntq0</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with sparky nails</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrntq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1jrns8p</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Cosmic brownie</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j33l3smd3wse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1jrnnrg</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>For all the bug loving baddies 💅🐜</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrnnrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1jrmx0a</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Milky white🤍</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm7jhgnlwvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1jrmwu2</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Bee-utiful! 🐝</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2b2bi6ojwvse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1jrm4t8</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Got inspiration from this channel for these!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08fgtgolqvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1jrme3g</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Season</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqtaa52msvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1jrmbga</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Does this shape suit my hands?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq6p4c31svse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1jrm1o0</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>New Spring Mani</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrm1o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1jrlh3g</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>should I go back for a refund??</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrlh3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1jrlb0n</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>New Gel X set as a beginner</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mib799ibkvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1jrl4ep</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Leave them or add glitter?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pongx0h1jvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1jrl0mw</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Is this a bad nail job?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrl0mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1jrkrmm</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Recommended Nails For Guitar?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrkrmm/recommended_nails_for_guitar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1jrkpf1</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Ok..what now?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvu3vnovfvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1jrkjhh</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>💜 Painted Polish Gator Glitz 🐊 It's giving swamp witch vibes 💚</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3irqc5nevse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1jrjrev</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>I love these mixed glitter dips. Black makes them POP! In love with the pink and green.</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrjrev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1jri7vd</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>New set what do you all think? I love them 😍😁</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jri7vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1jrh78i</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>My fav set by far 🤭🧡</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fszgvn7ipuse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1jrhl3m</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>I stick paper under my nail bed to detach it and then cut it into a reverse triangle piece</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrhl3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1jrhjzh</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I did my best friends nails what do you think?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rps8ifa4suse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1jrajsi</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Why does my thumb nail divot at the tip when it grows in? The same doesn’t happen to my other thumb.</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wij5jj6l9tse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1jr93zg</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Extremely broken nail and an unhappy client, advice?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jr93zg/extremely_broken_nail_and_an_unhappy_client_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1jr9z1g</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>need help!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr9z1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1jrbf94</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>First press-ons ever. I have worries and questions?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrbf94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1jrffb5</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Why does my mani keep doing this?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrffb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1jrg6dq</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>What’s happening with my nails?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg87vlexhuse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1jrgbz5</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>New to press-ons, any advice?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrgbz5/new_to_pressons_any_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1jrgr3x</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Apple nails</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrgr3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1jrgno4</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Mushroom garden 🍄‍🟫</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnjxmykgluse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1jr8frk</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I want to give my technician a shoutout</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr8frk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1jrfm7g</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>My Birthday nails this year 🌙☀️</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrfm7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1jrgh8e</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>My ombre glitter nails.</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhk4vrw4kuse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1jrgesu</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Odd White spots on both of my thumbs?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrgesu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1jr4xfs</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Wedding Nails - Emergency Fixes</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jr4xfs/wedding_nails_emergency_fixes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1jr9n4k</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Gel x fill in</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg1rgvm80tse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1jrbl4u</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Mini eggs nails for Easter</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbrss8klitse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1jrdc53</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Should I just switch to glue?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jrdc53/should_i_just_switch_to_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1jrykbe</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>7 day wear of new Essie Gel Couture formula</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrykbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1jrxg8g</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Attempting a Hard Candy Frigid look</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrxg8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1jrxdfm</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Bug nails 🪲🐞🐛💅</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrxdfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1jrw7s7</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Help!!  Polish brands with the *most-transparent* jellies?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrw7s7/help_polish_brands_with_the_mosttransparent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1jrw6wr</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer- The Human Condition</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrw6wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1jrvgjk</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Lurid lacquer Why Not Both</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrvgjk/lurid_lacquer_why_not_both/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1jrumtx</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Finally swatched my polish collection!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daau7fabuxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1jrtavt</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Recommend Local/Drugstore Glossy QDTC</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrtavt/recommend_localdrugstore_glossy_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1jrsmw9</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I was sent here by bitches with taste to ask about these nonexistent nails and would love your help</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrs305</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1jrskvv</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Finally swatched my polishes</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrskvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1jrscra</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I was influenced…</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bri6m37g7xse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1jrs98x</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Purple aura nails to go with my grandmother's ring 💜</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4bcl8bk6xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1jrs43w</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>What's happening here?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9kiu6s25xse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1jrr9rv</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>So off season, so pretty</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrr9rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1jrr1f1</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Thank you all for sharing your wisdom - I'm finally getting good!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrr1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1jrqnfh</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Any Dupes for Odette?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrqnfh/any_dupes_for_odette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1jrqlkd</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>I'll take another dozen, please</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1o7o92cqwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1jrql0u</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Dazzle Dry french tip colors for a total newbie</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrql0u/dazzle_dry_french_tip_colors_for_a_total_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1jrq9sp</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>THE (STRUG)GLOW IS REAL - my own polish attempt, lol!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e45qaafklwse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1jrq9r6</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Love mooncat and in need of basecoat</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrq9r6/love_mooncat_and_in_need_of_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1jrq7i5</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>UK indie websites that aren't RC</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrq7i5/uk_indie_websites_that_arent_rc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1jrq1ku</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>was skeptical a green would look good on me—i LOVE this one 💚</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrq1ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1jrpr65</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>What ingredient in this body oil is "melting" my nail polish?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab35qp31jwse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1jrplb9</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Leave a Light On - EdM</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrplb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1jrp1xn</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Glowstick</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1izgc95sdwse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1jrofzg</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>contact dermatitis</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrofzg/contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1jrofg2</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Firefox over Earth to Gaia</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrofg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1jrodmc</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>As pink as petals 🌸</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrodmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1jro6k8</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>First attempt at strawberry milk nails</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jro6k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1jrnkiv</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Looking for these remover pads?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://a.co/d/cjdTSNEce.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1jrngwg</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>glowy blue pigment like ‘Nice Day for a Cardigan?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrngwg/glowy_blue_pigment_like_nice_day_for_a_cardigan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1jrn4tm</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>PPU Disaster</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrn4tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1jrn3vq</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>In love with the subtle shimmer</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrn3vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1jrmwln</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Zoya Yvonne</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrmwln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1jrmt5o</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Protest nails anyone? 🎉</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/efp9apvqvvse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1jrmljm</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>So clearly I’m a red girl…</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2dscfl5uvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1jrmjo5</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>When they get the shade name just right</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xtn3kc8otvse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1jrm8a2</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>My nails get these growth lines</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhz5xd7crvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1jrl4pn</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Maelstrom over Wavelength</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lw642ja3jvse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1jrkzn5</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Some Dark Blue Comparisons because I’m bored…</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrkzn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1jrky3q</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Well that sucks</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9ncdul4hvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1jrkais</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Anti-FOMO</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrkais/antifomo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1jrk7yo</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>💜 Painted Polish Gator Glitz 🐊 It's giving swamp witch vibes 💚</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5py2bj6cvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1jrhjrr</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I didnt expect just how much Mojo changes with lighting</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrhjrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1jrhebq</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>What polish looks the most  like burnished gold?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lusc6s2yquse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1jrh2eo</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Pink glazed chrome 🍩</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrh2eo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1jrgo0w</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>The Shag 🌿</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrgo0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1jrgml7</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Question from a Luminary newbie!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqlj0r59luse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1jrg8ub</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>So fresh and so cleannn</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hdsknpociuse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1jrfqrs</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Spoonful of Sugar🍬🍭</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bg341tmpeuse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1jrfn38</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Nature nails 🌿</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrfn38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1jrfivt</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Ordering Cirque Colors from Nailland.hu - brush question</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrfivt/ordering_cirque_colors_from_naillandhu_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1jrfcro</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with a holo glitter for spring!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csdpfr4vbuse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1jrf3ry</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I Did It!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrf3ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1jrf05f</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Unintentionally Seasonal Mani</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjt7c1h69use1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1jrenaj</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>🩷💜 Loving this thermal</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrenaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1jrek1x</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>I'm newly obsessed with kbshimmer</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a3ft3j9u5use1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1jregx1</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Fairy nails 🧚🏾‍♂️✨️🦋</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jregx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1jre6zr</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Underwhelmed by Curiosity's Prey</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gh1tkre63use1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1jre1pq</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>"Jazz" Nail Art</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jre1pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1jrdi9u</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>when the formula is just right 🤌🏻</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3386jz8xvtse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1jrdeh4</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>No mooncat at hypnoticpolish anymore :(</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bce89w9xtse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1jrdegd</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell is GORGEOUS.</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl39lxn9xtse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1jrd4ng</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Another Spring, another Safety Reminder</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrd4ng/another_spring_another_safety_reminder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1jrcwj0</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>If I paint a spring mani then spring weather will finally come, right?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrcwj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1jrcvcy</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>HT flaky jellies. I am a magpie</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icupzgh8ttse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1jrc7z2</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Results of layering ILNP Flower Child over a pink creme</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrc7z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1jrbu9o</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Peely Base &amp; Treatment?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/1jqww9r/peely_base_treatment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1jrbqiz</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Base Coat Battle 7</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrbqiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1jrb51f</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Polish that will stay on after working??</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrb51f/polish_that_will_stay_on_after_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1jra2us</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Need help with major shrinkage issues!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jra2us/need_help_with_major_shrinkage_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1jr9l8g</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Haven't seen this shade since... ever?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apvqh0500tse1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1jr8n3e</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Cajun Shrimp 🍤 Drama?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://theeverygirl.com/opi-cajun-shrimp-shade-change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1jqpbjp</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Help me find my dream green shade</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrlbi08fsnse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1jqqnzw</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>How to improve my French manicure?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jqqnzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1jqs35k</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Opinions on Thunder By Vanessa Molina (8th Anniversary Collection)?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jqs35k/opinions_on_thunder_by_vanessa_molina_8th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1jr1xje</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Tiger’s Eye Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/706kheavhqse1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1jr4gxg</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>OPI Pedal Faster Suzi Dupes?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr4gxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1jr74q8</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Newbie here!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwkh1x1n5sse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1jrwqr6</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Self-Nail Art - Best color for wedding nails?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jrwqr6/selfnail_art_best_color_for_wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1jrvod9</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Aldi😂</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu3zn8ze5yse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1jrv0k0</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2w0oz2ayxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1jrulpi</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>A dream of spring 🌼</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyn6h310uxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1jrsmw0</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Everyone decided to do fruit nails today</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrsmw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1jrq4et</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Cutesy, fruity, and nostalgic</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrq4et</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1jrpzny</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esl8tsuqlwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1jrpter</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>What are these??</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/mtLX2vb2I98?si=_5EUMuUOh1w6AcBE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1jroixd</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Before you say it’s too early- I live in FL 😅🌴</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jroixd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1jrnmhv</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>For all the bug loving baddies 💅🐜</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrnmhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1jrlrdg</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Daisies and blue skies for spring 🩵</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6xnh1pqnvse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1jrjwyy</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>What vibe do these give ?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3ov5wtu9vse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1jrd2u5</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Inspired by rednote nails ⭐️</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfjgjixrutse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1jrbc8m</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Mi primer trabajo, alguna sugerencia? ☺️</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhxjpwxpgtse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1jr9bpv</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I wanted to give my nail tech the credit she deserves</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jr9bpv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr  6 08:09:59 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_06.xlsx
+++ b/data/collected_data/2025_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1268"/>
+  <dimension ref="A1:C1461"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21989,6 +21989,3287 @@
         </is>
       </c>
     </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1jsp22f</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Pink swirls 💖</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsp22f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1jsoqgj</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Are these almond shaped or soft stiletto?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn7lpz8u36te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1jsopn4</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Flowers for Spring 🌸</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsopn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1jsogjt</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>First time working with 3D gel 💖</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsogjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1jso08g</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Question about customer etiquette when asking for short nails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jso08g/question_about_customer_etiquette_when_asking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1jsn415</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Are these too girly/immature?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9oi94xckj5te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1jsmsup</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>New nails 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsmsup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1jsmc7l</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I hate my nails what can i do?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsmc7l/i_hate_my_nails_what_can_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1jsmazb</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>I love it!🥰</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsmazb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1jsm9u2</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>5th DIY set with builder gel!</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odh51ufu95te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1jsm1fn</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>got my nails done today 😌</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gya1g8775te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1jslete</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Are these too flat?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jslete</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1jslfo0</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Social Media for Nail Techs</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jslfo0/social_media_for_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1jsldnr</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First time at home gel-X!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsldnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1jsl1do</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>In My Chrome Era</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvl1hrd9w4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1jsl07w</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Dual Color Shift Cateye—Real?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsl07w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1jskual</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Cat eye try #2!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8xjxfa6u4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1jsknfo</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>French tip with lavender base!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsknfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1jsjkkb</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Tips for nail maintenance?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdedqaw0h4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1jsjgy4</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>How do you choose nails for a multi-day event?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsjgy4/how_do_you_choose_nails_for_a_multiday_event/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1jsjw2s</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2t0ohnck4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1jsjs89</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>first post here - enjoying mooncat's "antifragile"!💜✨</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i799po4mh4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1jsja4n</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Self nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvotk2g5e4te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1jsi384</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Trying to feel out what nails I want to do for honeymoon in June 🌺🌴</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clixskaf24te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1jsisk5</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>DND Red Cherry 🍒</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsisk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1jsio0b</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Loving the holo purple</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu5ie6sy74te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1jsilto</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Rapunzel Themed</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ory5f7oe74te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1jsihkc</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d349zpb864te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1jsihj1</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>questions about shellac</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsihj1/questions_about_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1jsi0xl</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Game Day means Nail Day</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsi0xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1jshsos</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Spent pretty much the entire day on these</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wc4wah5oz3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1jshrw5</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Wedding in a week, nail question</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jshrw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1jsh896</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>How in the hell do nail techs manage walk-ins, and appointments and doing manicures and pedicures for like a group of 4?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsh896/how_in_the_hell_do_nail_techs_manage_walkins_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1jsheg7</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>My beautiful spring in Japan inspired nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsheg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1jshgg1</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upyb40mhw3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1jshl0n</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>How often do you get your nails done?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jshl0n/how_often_do_you_get_your_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1jsh8j1</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Upturned Gel Manicures</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsh8j1/upturned_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1jsh4hp</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Celestial ✨ 🌙 ☀️</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkhqyxqgt3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1jsgvq4</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>A spring gel for all my dudes out there</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yzimkh8r3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1jsgpaz</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Price of gel nails in Sydney? Am I paying too much?</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsgpaz/price_of_gel_nails_in_sydney_am_i_paying_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1jsgds0</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸🌿</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsgds0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1jsgbu0</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3df536k9m3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1jsg7la</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Trying out square nails 💖</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsg7la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1jsfzoq</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Alternatives to Japanese gel</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsfzoq/alternatives_to_japanese_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1jsfyk3</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we6e4em3j3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1jsf353</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>How to extend length without common allergens</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jsf353/how_to_extend_length_without_common_allergens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1jsex31</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Why does my nail polish look burnt?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsex31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1jsfcyh</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Indecisive</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/057ocawsd3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1jsf3ze</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>First time doing my nails in years ! 🦎</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18g7sxyqb3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1jseybi</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Top Coats</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jseybi/top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1jseq2a</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Mother and Daughter Nail Therapy.</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jseq2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1jsdoo5</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Help!! Curved nail</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsdoo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1jseged</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Simply lovely</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy70zbk863te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1jsebog</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Diy Gels</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqfhbr6553te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1jsebul</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Just got them done</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3le6op653te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1jsdwsp</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ffn8v9q13te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1jsdvwj</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Beetles Pearl Gel</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81qcsrgj13te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1jsdnk4</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>i am so in love but my friend says its not good</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdbfw7tnz2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1jsdh6t</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>I love them, and you? 💅</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcoegzd9y2te1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1jsd54c</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Am I overreacting ?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xo2evlxgv2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1jsd5vz</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>For my jungle trip. I used random inspo from multiple Pinterest photos. The second picture was the first try, but I didn’t like the ring finger. Now, I’m just wondering if the index ties in okay. Or should I change it?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsd5vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1jsd36s</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Cat eye, glitter, chrome, and flowers 🌸</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsd36s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1jscz0u</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Do you like being a nail artist?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbt7vcw9u2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1jscctw</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Money Nails 💰</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jscctw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1jsc9pl</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>How do I actually do my nails? Do I have to have press ons to get this shape or is there something I can do with my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jLsdNKg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1jsbxdm</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Recreating the look of horsehair raku pottery on fingernails? Is it possible?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuc0umg4m2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1jsbn9l</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>How do I smooth out my nails and not make them look so crusty lol</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v9mw7puj2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1jsbj1d</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What color is Selena Gomez nails 💅 on her ig story?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flcbmc4wi2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1jscex8</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jscex8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1jsce4a</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>3D Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsce4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1jscd7u</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>First Time w/Gel X</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l0m83ryo2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1jsbklt</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>After months of the same nude color…I decided to brighten it up a bit (still doesn’t beat nude though 😂)</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsbklt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1jsb2xb</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Chrome French Tips</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsb2xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1jsam4c</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Spring Set!</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsam4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1jsak09</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>My new nails 😌</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsak09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1jsaipn</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>were these worth it?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsaipn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1jsai0w</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Builder Gel Nail Lifting</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mxb29mya2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1js7gvr</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>How do I get more traction on instagram as a student nail tech?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js7gvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1js660c</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Water Lilies 🪷 inspired by a Juan Del Pozo painting (found on the Eclectic Gallery London website)</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js660c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1js5d8q</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Sring inspired 🍃</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxkenyhk61te1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1js25qr</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Quick question about dip nails</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1js25qr/quick_question_about_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1jryov9</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Any recommendations for ridge filler nail polish? In UK</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jryov9/any_recommendations_for_ridge_filler_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1jrtso2</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Help me find this color please!!</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itki8zzplxse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1js785w</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>How do y'all make the patterns and designs on your nails so flawlessly?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1js785w/how_do_yall_make_the_patterns_and_designs_on_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1js7jpq</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Removing press ons without damage?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1js7jpq/removing_press_ons_without_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1js9xbr</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Please convince me these look good🥲</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9xbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1js9mfl</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>my nails and the inspo</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9mfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1js9lws</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a polish with this color?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9lws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1js8jqz</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>I am cat-eye obsessed!</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js8jqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1jsae1s</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>No more black did make me feel more uplifted</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsae1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1jsa7v6</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Got a new color and was excited to try it ☺️ 💙</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xgj6gis82te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1jsa6if</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>I sat on this set of temperature changing polishes because I thought the color mixes weren't for me and then it turns out they are and as a bonus it looks like it's chromed on top of it!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2d0bd4i82te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1js9ue9</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Summer is here!</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdjpaq8w52te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1js9rmz</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Could I become a hand model?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9rmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1js9q4e</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>advice for keeping nails clean/in good condition while having a job i get dirty</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9q4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1js9loi</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Raw Amethyst</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv7gbaj142te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1js9i28</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Growing out nails, need tips</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9i28</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1js90xb</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>question - regular gel manicure after prolonged builder gel manicures?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1js90xb/question_regular_gel_manicure_after_prolonged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1js8yg4</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Thermal nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8m10d3kxy1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1js8fuy</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Rate my new nails 🎀🤍✨</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmueprw0v1te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1jsmyw2</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Brought out my favorite yellow of all time, alongside the iconic Cock-a-doodle Doom</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntkefjbuh5te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1jsl4co</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>ISO a comparison of ILNP pine and Essie off tropic</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jsl4co/iso_a_comparison_of_ilnp_pine_and_essie_off_tropic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1jskoq2</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Fitbit misreading heart rate when painting nails?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jskoq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1jsknsj</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>welcome to stardew valley 🌱🐓</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/70l8ewybs4te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1jsk79i</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Mooncat After the Rain and ILNP Bluebell layer</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kgat1pekn4te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1jsj454</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Blade of the frontiers</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsj454</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1jsiu1g</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Battlestation for a small apartment</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsiu1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1jsik5k</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>First time trying blooming gel!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61mpfi8y64te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1jsihfn</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Trying out nail art</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsihfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1jsiby9</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>This sub has altered my brain.</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ajuroiq44te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1jshr20</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Look at this shift!!</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cft6zx49z3te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1jsh9mp</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>TY for the magnet tips 💜</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hedyscqru3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1jsh5hi</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Color Club</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsh5hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1jsh1cd</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>I really, really like green.💚</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/berm98ens3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1jsgjoa</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>i need some nail care advice!!</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsgjoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1jsgjdl</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>KBShimmer Sea-ing is Believing</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsgjdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1jsgblu</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>New mani - a little more spring like than my usual</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsgblu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1jsg682</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Some OPI Funny Bunny</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnjlvokwk3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1jsfeq7</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Surprise combo!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsfeq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1jsexq1</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>I had a vision. I halfway achieved it 🙃</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsexq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1jseoeh</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Strawberry Cheesecake</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jseoeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1jseaxh</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>We've been sleeping on Entanglemint!</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nmyz4ia833te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1jse9nb</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>got a particularly nice photo</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhkhsh4o43te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1jsdr4i</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Pleasantly surprised</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsdr4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1jsdlam</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>In love with how the flakes reflect the light</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trt7ht76z2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1jsdgfp</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Distance to the Sun</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsdgfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1jsdesj</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer's Prototype 260</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsdesj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1jsdepj</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Why is did the color get muddy?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75s5udcpx2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1jsd1xg</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>How do y’all take such nice pics of your nails?😭</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsd1xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1jscrgj</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>ILNP Abundance and hot take on MC Maelstrom</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jscrgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1jsckwz</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My first butterfly nails (creative, i know 😆🦋)</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsckwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1jscjv9</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Obsessed 🥰💅</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73wm7ef0r2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1jsbypo</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>BKL-Only One Bed</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fvn3uj0fm2te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1jsbqgq</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>I found a real ladybug to go with my bug nails 🐞</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsbqgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1jsb2kg</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Hands Off!</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bkkq59cf2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1jsap8m</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>I wore only pink polish for February</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsap8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1jsagt9</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Bisou Bisou then &amp; now (1 year)</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsagt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1jsa9na</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Applying cheap black cremes with my non dominant hand is the most stressful.</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsa9na</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1jsa7hd</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Psilocin blows my mindsilocin.</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsa7hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1js9u7q</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Olive and June Polish Remover Pot</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/je5ph9ou52te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1js9lby</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Root of All Evil by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ozh36czu32te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1js9e9w</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Tyler Trinket's New Collection: G-Ray of Sunshine, combines moody gray bases with a hint of silver sparkle and a vibrant aurora shimmer</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://tylerstrinkets.com/collections/g-ray-of-sunshine</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1js9ao0</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Color match my car!</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js9ao0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1js8ypq</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>🖤🔥🌈 Lacquer Tutorial</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j8h4z6j2y1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1js8tal</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>The color shift is ridiculous! I think I have a new favorite nail polish!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tcuyex1xx1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1js8idh</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>I am cat-eye obsessed!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js8idh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1js8esc</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>One and only, Fairy Dust 🧚🏼‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js8esc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1js8ds6</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Awfully Pond of You🐸🪷</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7hriv36ju1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1js8c3q</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>ILNP - Hex</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js8c3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1js7jfi</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Your Favourite Polishes that No One Talks About</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1js7jfi/your_favourite_polishes_that_no_one_talks_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1js7g7a</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Boos &amp; Cats</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js7g7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1js7a1v</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Obsessed with combining soft magnetics and shimmers</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js7a1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1js76qr</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Velvet? For a Magnetic Polish? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fzgypb09l1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1js6ugu</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>I have no words.</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g5da6quji1te1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1js6tiy</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Come on, spring… ready for you! 🌺🌷💐🌸🌹</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tbml9xci1te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1js5xdk</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>First time posting a mani 💅</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js5xdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1js5r6m</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Nail Polish sitting in mail box for 2 full 80⁰F days</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1js5r6m/nail_polish_sitting_in_mail_box_for_2_full_80⁰f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1js5mgc</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>These kept distracting me during workout~🐲</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js5mgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1js559s</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>New favourite colour!</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js559s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1js52nn</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Birthday neon nails</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js52nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1js4o07</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Help me narrow down my cart please!!</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js4o07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1js3z89</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>L.A. Colors- Be Mine🌹</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js3z89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1js3miv</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Help finding a polish for my kid please!</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1js3miv/help_finding_a_polish_for_my_kid_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1js3mdc</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>I’m Never Taking This Off!!!!</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoahnkior0te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1js2taw</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Help with IDing this shade please!!</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vv56stck0te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1js2k23</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Am ninja. Successfully touched up nails on moving London Underground carriage</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah32zq0ph0te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1js2hs1</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Restoration Help</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12h96lw5h0te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1js1a4j</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Pls help find the "Grandmaster blue"</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qay389920te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1js0jtd</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Not the cleanest mani, but I love this look 🦋🦋</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uni3xkq8vzse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1js08pf</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Proximal nail fold is detached but not painful</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js08pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1jrqwdv</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>OPI Wicked “ Ga-Linda”</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21vfvngttwse1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1jrzggg</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>I heared we are showing off our collection? 👀(Bonus mani)</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jrzggg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1jrynlq</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Pop•Arazzi white &amp; pastel colors</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jrynlq/poparazzi_white_pastel_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1jsnhat</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Help! What is happening to my nails.</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsnhat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1jsmvkw</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Minecraft nails</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsmvkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1jsksz4</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Oranges and Folk Art</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsksz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1jskpyj</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Peeps anyone? Easter nails!</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jskpyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1jsiknv</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Rapunzel Themed</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs5079b374te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1jsgbqe</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>What color is this?</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl4jr3q8m3te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1jse9hd</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>What do we think about reverse chrome isolation</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw0ikl4n43te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1jse4yq</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>I think it’s a Christmas desim😂</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3qv3kbl33te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1jscqeg</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Best brushes for fine lines?</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jscqeg/best_brushes_for_fine_lines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1jscg5l</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>It’s a process!!!!</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jscg5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1jsc9of</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Money Nail Art 💵</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsc9of</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1jsb8wa</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Flores</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1oyp9xog2te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1jsao1f</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Gorgeous spring nails with gold accents. Done @ Phillynails by @sueznails on ig. They’re not on Reddit so can’t credit them on here</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jsao1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1js8fk4</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Just finished up nail school and these are my first attempts at nail art. Stickers, hand painted, foils and glitter 😅</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js8fk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1js7lig</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>White Lotus Nail Art</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js7lig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1js6gt8</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Frog nails on shorties</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kifkkubjf1te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1js5kor</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>New nail art! Constructive criticism welcome</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js5kor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1js444f</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Amo el color rojo mis amores ♥️♥️♥️</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biej4233w0te1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1js3ie6</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Minecraft nails with Lizzie and Joel!</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js3ie6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1js1lu6</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Glittery flowers ✨</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1js1lu6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>